<commit_message>
an hanh from leader
</commit_message>
<xml_diff>
--- a/quanlytong/export.xlsx
+++ b/quanlytong/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>mstu</t>
   </si>
@@ -23,103 +23,22 @@
     <t>mskhungtu</t>
   </si>
   <si>
-    <t>000000000011</t>
-  </si>
-  <si>
-    <t>00000000001101</t>
-  </si>
-  <si>
-    <t>00000000001102</t>
-  </si>
-  <si>
-    <t>00000000001103</t>
-  </si>
-  <si>
-    <t>00000000001104</t>
-  </si>
-  <si>
-    <t>00000000001105</t>
-  </si>
-  <si>
-    <t>000000000012</t>
-  </si>
-  <si>
-    <t>00000000001201</t>
-  </si>
-  <si>
-    <t>00000000001202</t>
-  </si>
-  <si>
-    <t>00000000001203</t>
-  </si>
-  <si>
-    <t>00000000001204</t>
-  </si>
-  <si>
-    <t>00000000001205</t>
-  </si>
-  <si>
-    <t>00000000001206</t>
-  </si>
-  <si>
-    <t>00000000001207</t>
-  </si>
-  <si>
-    <t>00000000001208</t>
-  </si>
-  <si>
-    <t>00000000001209</t>
-  </si>
-  <si>
-    <t>00000000001210</t>
-  </si>
-  <si>
-    <t>000000000013</t>
-  </si>
-  <si>
-    <t>00000000001301</t>
-  </si>
-  <si>
-    <t>00000000001302</t>
-  </si>
-  <si>
-    <t>00000000001303</t>
-  </si>
-  <si>
-    <t>00000000001304</t>
-  </si>
-  <si>
-    <t>00000000001305</t>
-  </si>
-  <si>
-    <t>00000000001306</t>
-  </si>
-  <si>
-    <t>00000000001307</t>
-  </si>
-  <si>
-    <t>00000000001308</t>
-  </si>
-  <si>
-    <t>00000000001309</t>
-  </si>
-  <si>
-    <t>00000000001310</t>
-  </si>
-  <si>
-    <t>00000000001311</t>
-  </si>
-  <si>
-    <t>00000000001312</t>
-  </si>
-  <si>
-    <t>00000000001313</t>
-  </si>
-  <si>
-    <t>00000000001314</t>
-  </si>
-  <si>
-    <t>00000000001315</t>
+    <t>111111111001</t>
+  </si>
+  <si>
+    <t>11111111100101</t>
+  </si>
+  <si>
+    <t>11111111100102</t>
+  </si>
+  <si>
+    <t>11111111100103</t>
+  </si>
+  <si>
+    <t>11111111100104</t>
+  </si>
+  <si>
+    <t>11111111100105</t>
   </si>
 </sst>
 </file>
@@ -458,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,206 +431,6 @@
       </c>
       <c r="B6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>